<commit_message>
Added Graphs for 4 more columns
</commit_message>
<xml_diff>
--- a/data/OutputTemplate.xlsx
+++ b/data/OutputTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlkg\PycharmProjects\TSUSPTMDATA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlkg\Downloads\Programing\SPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBE8B1-5D87-4469-A98B-61915933B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D26B6F-0B06-478F-A1F5-2A8CF625BFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -264,6 +263,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -599,6 +628,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1233,6 +1292,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1278,6 +1367,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1323,6 +1442,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1368,6 +1517,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1413,6 +1592,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1458,6 +1667,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1505,6 +1744,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1552,6 +1821,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1599,6 +1898,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1646,6 +1975,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1661,6 +2020,316 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000009-78AD-40CF-B067-54073470F78E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-978E-4515-914F-0F0CE459F32C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$M$2:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-978E-4515-914F-0F0CE459F32C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$N$2:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-978E-4515-914F-0F0CE459F32C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-978E-4515-914F-0F0CE459F32C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1867,6 +2536,1466 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Counts!$L$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1C5-421A-9C38-6502174AC7BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1280347440"/>
+        <c:axId val="1280357280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1280347440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280357280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280347440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Counts!$M$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$M$2:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C884-46AB-91BF-335E23937B71}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1280347440"/>
+        <c:axId val="1280357280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1280347440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280357280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280347440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Counts!$N$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$N$2:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1315-4024-A8C0-3DAB2C96EA09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1280347440"/>
+        <c:axId val="1280357280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1280347440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280357280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280347440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Counts!$O$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-371C-440A-B191-61F6CE0A4C77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1280347440"/>
+        <c:axId val="1280357280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1280347440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280357280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280347440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -2021,6 +4150,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2366,6 +4525,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2701,6 +4890,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3036,6 +5255,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3371,6 +5620,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -3706,6 +5985,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4041,6 +6350,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4376,6 +6715,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -4688,6 +7057,166 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6557,6 +9086,2018 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11541,6 +16082,158 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29308</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>177034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3EEBD7-8F94-4A80-AC02-D964F71FC53C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>177034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81F01D73-2DC5-4DA8-9B51-3923604F645E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29308</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>177034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D664F762-A54B-4841-AF2F-E112C6F7B82F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>177034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="21" name="Chart 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E3E513B-0B47-45EE-84AC-A8CB459E01D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11843,8 +16536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6A69BA-E884-4881-977D-C690B88D8587}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11865,34 +16558,54 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
@@ -11905,16 +16618,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57A342-4862-437D-A083-E64B6B5A83A0}">
-  <dimension ref="C155"/>
+  <dimension ref="C178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155"/>
+    <sheetView topLeftCell="A142" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="K159" sqref="K159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C155" t="s">
+    <row r="178" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C178" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated profile and output template file
</commit_message>
<xml_diff>
--- a/data/OutputTemplate.xlsx
+++ b/data/OutputTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlkg\Downloads\Programing\SPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D26B6F-0B06-478F-A1F5-2A8CF625BFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4002869A-D407-41FC-90EB-0EC34FB4C3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
@@ -989,19 +989,19 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Counts!$B$1:$K$1</c:f>
+              <c:f>Counts!$B$1:$O$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Counts!$B$12:$K$12</c:f>
+              <c:f>Counts!$B$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="14"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -16536,7 +16536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6A69BA-E884-4881-977D-C690B88D8587}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -16620,7 +16620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57A342-4862-437D-A083-E64B6B5A83A0}">
   <dimension ref="C178"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="K159" sqref="K159"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 2 more plots
</commit_message>
<xml_diff>
--- a/data/OutputTemplate.xlsx
+++ b/data/OutputTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlkg\Downloads\Programing\SPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4002869A-D407-41FC-90EB-0EC34FB4C3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0D1C06-2C5C-496C-AB1E-57C564D042CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3996,6 +3989,736 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Counts!$O$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$P$2:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B648-4C06-9E92-ED44FCC28EE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1280347440"/>
+        <c:axId val="1280357280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1280347440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280357280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280347440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>Counts!$O$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$Q$2:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5793-43F0-9BC9-CEDC136C2434}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1280347440"/>
+        <c:axId val="1280357280"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1280347440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280357280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1280357280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1280347440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -7256,6 +7979,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11098,6 +11901,1012 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16234,6 +18043,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29308</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>177034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D10E1E48-BEEB-4164-8AD2-0AAF7616D4AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>177034</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E6F6DA-8893-43C8-9868-D17793BFF0D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16534,18 +18419,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6A69BA-E884-4881-977D-C690B88D8587}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -16556,58 +18441,64 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
     </row>
   </sheetData>
@@ -16618,16 +18509,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57A342-4862-437D-A083-E64B6B5A83A0}">
-  <dimension ref="C178"/>
+  <dimension ref="C204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K159" sqref="K159"/>
+    <sheetView topLeftCell="A157" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="K177" sqref="K177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="178" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C178" t="s">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C204" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added chart titles and updated json profile
</commit_message>
<xml_diff>
--- a/data/OutputTemplate.xlsx
+++ b/data/OutputTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlkg\Downloads\Programing\SPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0D1C06-2C5C-496C-AB1E-57C564D042CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFB9938-6FD8-4CF3-845D-E6BB88F87174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
@@ -4006,7 +4006,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Counts!$O$1</c:f>
+          <c:f>Counts!$P$1</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
           </c:strCache>
@@ -4371,7 +4371,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Counts!$O$1</c:f>
+          <c:f>Counts!$Q$1</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
           </c:strCache>
@@ -18421,16 +18421,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6A69BA-E884-4881-977D-C690B88D8587}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.59765625" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -18448,57 +18448,57 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
     </row>
   </sheetData>
@@ -18511,13 +18511,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57A342-4862-437D-A083-E64B6B5A83A0}">
   <dimension ref="C204"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="K177" sqref="K177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="204" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="204" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C204" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added new columns to chart and added Excel Macro to generate PPT
</commit_message>
<xml_diff>
--- a/data/OutputTemplate.xlsx
+++ b/data/OutputTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjlkg\Downloads\Programing\SPC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFB9938-6FD8-4CF3-845D-E6BB88F87174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9629F7A-F2C5-4E3A-A7BB-C7D628B6D0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{C3C02D5D-17E6-4691-A359-DBDA44FAC769}"/>
   </bookViews>
@@ -982,19 +982,19 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Counts!$B$1:$O$1</c:f>
+              <c:f>Counts!$B$1:$Q$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Counts!$B$12:$O$12</c:f>
+              <c:f>Counts!$B$12:$Q$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2323,6 +2323,162 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-978E-4515-914F-0F0CE459F32C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$P$2:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D35-4957-9C53-E682BC1EF73D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Counts!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Counts!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Counts!$Q$2:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D35-4957-9C53-E682BC1EF73D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17818,15 +17974,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>5233</xdr:colOff>
+      <xdr:colOff>40122</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>47104</xdr:rowOff>
+      <xdr:rowOff>54082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>125604</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>174451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17856,15 +18012,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47103</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>26166</xdr:rowOff>
+      <xdr:colOff>5235</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>179683</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596622</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57569</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>174450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>160495</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18511,8 +18667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57A342-4862-437D-A083-E64B6B5A83A0}">
   <dimension ref="C204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="K177" sqref="K177"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>